<commit_message>
Complete Ambient V0.3 Summary and Excel summary sheet
</commit_message>
<xml_diff>
--- a/SUMR25_Rockfish_Results_Summary_Table.xlsx
+++ b/SUMR25_Rockfish_Results_Summary_Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rmcke\OneDrive\Documents\Summer_2025_Rockfish_Research_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A6D0317-DA1F-414F-BFB7-ABC2C691F249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE82803-8FC3-46FB-B42F-B2E9BDD8EB1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C51F1DA1-53CD-44F2-AE8A-567F539ABD17}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="123">
   <si>
     <t>Parameter</t>
   </si>
@@ -261,14 +261,236 @@
   </si>
   <si>
     <t>Not Yet</t>
+  </si>
+  <si>
+    <t>Linear Model</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ambient Samples</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Testing: </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Differences between Fecundity Class</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ambient No Atresia Samples</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Testing: </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Corralation between Parameter and Weight Adjusted Fecundity</t>
+    </r>
+  </si>
+  <si>
+    <t>Significant Correlation</t>
+  </si>
+  <si>
+    <t>Aov(param ~ Fecundity_Class)</t>
+  </si>
+  <si>
+    <t>Aov Pr(&gt;F)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Low (~1,000s)-High (&gt;50,000) Tukey HSD p adj </t>
+  </si>
+  <si>
+    <t>Atresia-High (&lt;50,000) Tukey HSD p adj</t>
+  </si>
+  <si>
+    <t>Atresia-Low (~1,000s) Tukey HSD p adj</t>
+  </si>
+  <si>
+    <t>lm p-value</t>
+  </si>
+  <si>
+    <t>lm Adjusted R squared</t>
+  </si>
+  <si>
+    <t>lm Multiple R squared</t>
+  </si>
+  <si>
+    <t>DHARMA Errors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Significant Correlation after transformation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sqrt </t>
+  </si>
+  <si>
+    <t>lm(sqrt pH ~ weight_adj_fec)</t>
+  </si>
+  <si>
+    <t>lm(param ~ weight_adj_fec)</t>
+  </si>
+  <si>
+    <t>lm(sqrt param ~ weight_adj_fec)</t>
+  </si>
+  <si>
+    <t>Transformation Fix DHARMA Errors</t>
+  </si>
+  <si>
+    <t>0.021 *</t>
+  </si>
+  <si>
+    <t>??? Residuals qqplot looks good</t>
+  </si>
+  <si>
+    <t>Which Groups Different</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Atresia-Low</t>
+  </si>
+  <si>
+    <t>??? Residuals qqplot not great</t>
+  </si>
+  <si>
+    <t>Some quantile regressions failed</t>
+  </si>
+  <si>
+    <t>lm(sqrt Hct ~ weight_adj_fec)</t>
+  </si>
+  <si>
+    <t>Combine adjusted quantile test significant</t>
+  </si>
+  <si>
+    <t>??? Residual qqplot shows outlier</t>
+  </si>
+  <si>
+    <t>lm(sqrt Glu ~ weight_adj_fec)</t>
+  </si>
+  <si>
+    <t>Outlier Removed or Data transformed</t>
+  </si>
+  <si>
+    <t>Aov Pr(&gt;F) After outlier/transformation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Significant Difference after outlier/transformation </t>
+  </si>
+  <si>
+    <t>Attempted</t>
+  </si>
+  <si>
+    <t>Maybe</t>
+  </si>
+  <si>
+    <t>Quantile deviations detected (N.S.)</t>
+  </si>
+  <si>
+    <t>Met, but close (p-value = 0.09843)</t>
+  </si>
+  <si>
+    <t>??? Residual qqplot looks good</t>
+  </si>
+  <si>
+    <t>??? Residual qqplot shows some dev</t>
+  </si>
+  <si>
+    <t>Met, p-value = 0.1849</t>
+  </si>
+  <si>
+    <t>lm p-value after transfor/outlier removal</t>
+  </si>
+  <si>
+    <t>lm Multiple R-squared after trans/outlier rem</t>
+  </si>
+  <si>
+    <t>lm Adjusted R-squared after tans/out rem</t>
+  </si>
+  <si>
+    <t>0.00482 **</t>
+  </si>
+  <si>
+    <t>Atresia-High, Atresia-Low</t>
+  </si>
+  <si>
+    <t>No, p-value = 0.08147 (residuals of shapiro test)</t>
+  </si>
+  <si>
+    <t>No, passes Levene's</t>
+  </si>
+  <si>
+    <t>??? Residual qqplot shws outlier</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -638,11 +860,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE3A64F3-3469-4D7F-B2FA-BB9A0F539FC4}">
-  <dimension ref="A1:T10"/>
+  <dimension ref="A1:U34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M11" sqref="M11"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -651,13 +873,15 @@
     <col min="2" max="2" width="29.1796875" style="1" customWidth="1"/>
     <col min="3" max="3" width="29.81640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="34.6328125" customWidth="1"/>
-    <col min="5" max="5" width="22.54296875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="37.54296875" style="1" customWidth="1"/>
     <col min="6" max="6" width="33.26953125" style="1" customWidth="1"/>
-    <col min="7" max="8" width="25.6328125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="23.453125" customWidth="1"/>
+    <col min="7" max="7" width="31.90625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="32.81640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="38.81640625" customWidth="1"/>
     <col min="10" max="10" width="32.54296875" customWidth="1"/>
-    <col min="11" max="12" width="24.54296875" customWidth="1"/>
-    <col min="13" max="13" width="18.26953125" customWidth="1"/>
+    <col min="11" max="11" width="24.54296875" customWidth="1"/>
+    <col min="12" max="12" width="36.36328125" customWidth="1"/>
+    <col min="13" max="13" width="29.36328125" customWidth="1"/>
     <col min="14" max="14" width="31.36328125" customWidth="1"/>
     <col min="15" max="15" width="34" style="2" customWidth="1"/>
     <col min="16" max="16" width="40.1796875" customWidth="1"/>
@@ -666,7 +890,7 @@
     <col min="19" max="20" width="36.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -728,7 +952,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -769,7 +993,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -811,7 +1035,7 @@
       </c>
       <c r="N3" s="1"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -873,7 +1097,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -935,7 +1159,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -973,7 +1197,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1035,7 +1259,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1076,13 +1300,657 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>18</v>
       </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B14" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I16" t="s">
+        <v>22</v>
+      </c>
+      <c r="J16" t="s">
+        <v>21</v>
+      </c>
+      <c r="K16" t="s">
+        <v>25</v>
+      </c>
+      <c r="L16" t="s">
+        <v>38</v>
+      </c>
+      <c r="M16" t="s">
+        <v>105</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="O16" t="s">
+        <v>107</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="T16" t="s">
+        <v>22</v>
+      </c>
+      <c r="U16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="D17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0.90847259999999996</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0.59664039999999996</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0.31416110000000003</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0.21866269999999999</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0.61769870000000004</v>
+      </c>
+      <c r="H18" s="1">
+        <v>1.6265399999999999E-2</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="D19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0.96322099999999999</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0.3518867</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0.52779640000000005</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0.438</v>
+      </c>
+      <c r="D20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0.95264649999999995</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0.69391789999999998</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0.47374840000000001</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.92</v>
+      </c>
+      <c r="D21" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0.98473310000000003</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0.98015640000000004</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0.91700090000000001</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J21" t="s">
+        <v>33</v>
+      </c>
+      <c r="L21" t="s">
+        <v>14</v>
+      </c>
+      <c r="M21" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="D22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0.99019550000000001</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0.54496310000000003</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0.64525869999999996</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J22" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D23" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0.84509029999999996</v>
+      </c>
+      <c r="G23" s="1">
+        <v>1.0333999999999999E-2</v>
+      </c>
+      <c r="H23" s="1">
+        <v>4.3346500000000003E-2</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="J23" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B25" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B27" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D27" t="s">
+        <v>86</v>
+      </c>
+      <c r="E27" t="s">
+        <v>85</v>
+      </c>
+      <c r="F27" t="s">
+        <v>78</v>
+      </c>
+      <c r="G27" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" t="s">
+        <v>21</v>
+      </c>
+      <c r="I27" t="s">
+        <v>87</v>
+      </c>
+      <c r="J27" t="s">
+        <v>25</v>
+      </c>
+      <c r="K27" t="s">
+        <v>38</v>
+      </c>
+      <c r="L27" t="s">
+        <v>93</v>
+      </c>
+      <c r="M27" t="s">
+        <v>88</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="P27" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0.37009999999999998</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0.13519999999999999</v>
+      </c>
+      <c r="E28" s="1">
+        <v>-8.8990000000000007E-3</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I28" t="s">
+        <v>34</v>
+      </c>
+      <c r="J28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" t="s">
+        <v>90</v>
+      </c>
+      <c r="O28"/>
+      <c r="P28" s="2"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0.30270000000000002</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0.17480000000000001</v>
+      </c>
+      <c r="E29" s="1">
+        <v>3.7249999999999998E-2</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N29" t="s">
+        <v>101</v>
+      </c>
+      <c r="O29">
+        <v>0.26729999999999998</v>
+      </c>
+      <c r="P29" s="2">
+        <v>0.19950000000000001</v>
+      </c>
+      <c r="Q29">
+        <v>6.6030000000000005E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0.88749999999999996</v>
+      </c>
+      <c r="D30" s="1">
+        <v>3.62E-3</v>
+      </c>
+      <c r="E30" s="1">
+        <v>-0.16239999999999999</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I30" t="s">
+        <v>102</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M30" t="s">
+        <v>14</v>
+      </c>
+      <c r="N30" t="s">
+        <v>104</v>
+      </c>
+      <c r="O30">
+        <v>0.83540000000000003</v>
+      </c>
+      <c r="P30" s="2">
+        <v>7.783E-3</v>
+      </c>
+      <c r="Q30">
+        <v>-0.15759999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0.87009999999999998</v>
+      </c>
+      <c r="D31" s="1">
+        <v>4.8269999999999997E-3</v>
+      </c>
+      <c r="E31" s="1">
+        <v>-0.161</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="I31" t="s">
+        <v>100</v>
+      </c>
+      <c r="N31" t="s">
+        <v>92</v>
+      </c>
+      <c r="O31"/>
+      <c r="P31" s="2"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32" s="1">
+        <v>0.87909999999999999</v>
+      </c>
+      <c r="D32" s="1">
+        <v>4.1799999999999997E-3</v>
+      </c>
+      <c r="E32" s="1">
+        <v>-0.1618</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="N32" t="s">
+        <v>92</v>
+      </c>
+      <c r="O32"/>
+      <c r="P32" s="2"/>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0.39</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0.12509999999999999</v>
+      </c>
+      <c r="E33" s="1">
+        <v>-2.069E-2</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I33" t="s">
+        <v>102</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="M33" t="s">
+        <v>34</v>
+      </c>
+      <c r="N33" t="s">
+        <v>92</v>
+      </c>
+      <c r="O33">
+        <v>0.37830000000000003</v>
+      </c>
+      <c r="P33" s="2">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="Q33">
+        <v>-1.3820000000000001E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C34" s="1">
+        <v>6.0060000000000002E-2</v>
+      </c>
+      <c r="D34" s="1">
+        <v>0.4713</v>
+      </c>
+      <c r="E34" s="1">
+        <v>0.3831</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="I34" t="s">
+        <v>102</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="N34" t="s">
+        <v>92</v>
+      </c>
+      <c r="O34"/>
+      <c r="P34" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add on new pCO2 param
</commit_message>
<xml_diff>
--- a/SUMR25_Rockfish_Results_Summary_Table.xlsx
+++ b/SUMR25_Rockfish_Results_Summary_Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rmcke\OneDrive\Documents\Summer_2025_Rockfish_Research_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE82803-8FC3-46FB-B42F-B2E9BDD8EB1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD8E43DC-D5C0-42C0-8A48-58F371858DD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C51F1DA1-53CD-44F2-AE8A-567F539ABD17}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="125">
   <si>
     <t>Parameter</t>
   </si>
@@ -141,9 +141,6 @@
   </si>
   <si>
     <t>No</t>
-  </si>
-  <si>
-    <t>Not Yet (original result stat values)</t>
   </si>
   <si>
     <t>p adj = 0.4134193</t>
@@ -337,9 +334,6 @@
     <t>Significant Correlation</t>
   </si>
   <si>
-    <t>Aov(param ~ Fecundity_Class)</t>
-  </si>
-  <si>
     <t>Aov Pr(&gt;F)</t>
   </si>
   <si>
@@ -467,6 +461,18 @@
   </si>
   <si>
     <t>??? Residual qqplot shws outlier</t>
+  </si>
+  <si>
+    <t>pCO2</t>
+  </si>
+  <si>
+    <t>aov(param ~ Fecundity_Class)</t>
+  </si>
+  <si>
+    <t>Met, p-value = 0.3922</t>
+  </si>
+  <si>
+    <t>0.0463 *</t>
   </si>
 </sst>
 </file>
@@ -860,11 +866,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE3A64F3-3469-4D7F-B2FA-BB9A0F539FC4}">
-  <dimension ref="A1:U34"/>
+  <dimension ref="A1:U36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O34" sqref="O34"/>
+    <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -925,143 +931,136 @@
         <v>25</v>
       </c>
       <c r="L1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M1" t="s">
         <v>24</v>
       </c>
       <c r="N1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Q1" t="s">
+        <v>45</v>
+      </c>
+      <c r="R1" t="s">
         <v>46</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>47</v>
       </c>
-      <c r="S1" t="s">
-        <v>48</v>
-      </c>
       <c r="T1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>121</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>26</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.94059999999999999</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>19</v>
+        <v>124</v>
       </c>
       <c r="F2" s="1">
-        <v>4.8339999999999998E-3</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>20</v>
+        <v>4.6259500000000002E-2</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.1007</v>
       </c>
       <c r="H2" s="1">
-        <v>2.6428E-2</v>
+        <v>0.1018949</v>
       </c>
       <c r="I2" t="s">
         <v>33</v>
       </c>
       <c r="J2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" t="s">
         <v>34</v>
       </c>
       <c r="L2" t="s">
-        <v>14</v>
-      </c>
-      <c r="M2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0.87150000000000005</v>
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0.24510000000000001</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="1">
+        <v>4.8339999999999998E-3</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="1">
+        <v>2.6428E-2</v>
+      </c>
+      <c r="I3" t="s">
         <v>33</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>16</v>
+      <c r="J3" t="s">
+        <v>23</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="N3" s="1"/>
+      <c r="L3" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="C4" s="1">
-        <v>6.7100000000000007E-2</v>
+        <v>0.87150000000000005</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0.41339999999999999</v>
+        <v>28</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G4" s="1">
-        <v>0.38769999999999999</v>
+        <v>0.24510000000000001</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>16</v>
@@ -1070,63 +1069,43 @@
         <v>34</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="P4">
-        <v>0.64159999999999995</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>49</v>
-      </c>
-      <c r="R4">
-        <v>0.11210000000000001</v>
-      </c>
-      <c r="S4" t="s">
-        <v>50</v>
-      </c>
-      <c r="T4" t="s">
-        <v>54</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="N4" s="1"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1">
-        <v>0.24199999999999999</v>
+        <v>6.7100000000000007E-2</v>
       </c>
       <c r="D5" t="s">
         <v>34</v>
       </c>
       <c r="E5" s="1">
-        <v>0.37</v>
+        <v>0.41339999999999999</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G5" s="1">
-        <v>0.251</v>
+        <v>0.38769999999999999</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>34</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>34</v>
@@ -1135,182 +1114,244 @@
         <v>14</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="P5">
-        <v>0.52949999999999997</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>52</v>
+        <v>0.64159999999999995</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>48</v>
       </c>
       <c r="R5">
-        <v>0.10580000000000001</v>
+        <v>0.11210000000000001</v>
       </c>
       <c r="S5" t="s">
+        <v>49</v>
+      </c>
+      <c r="T5" t="s">
         <v>53</v>
-      </c>
-      <c r="T5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C6" s="1">
-        <v>0.67800000000000005</v>
+        <v>0.24199999999999999</v>
       </c>
       <c r="D6" t="s">
         <v>34</v>
       </c>
       <c r="E6" s="1">
-        <v>0.753</v>
+        <v>0.37</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="G6" s="1">
-        <v>0.46700000000000003</v>
+        <v>0.251</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>34</v>
+        <v>14</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="P6">
+        <v>0.52949999999999997</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R6">
+        <v>0.10580000000000001</v>
+      </c>
+      <c r="S6" t="s">
+        <v>52</v>
+      </c>
+      <c r="T6" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C7" s="1">
-        <v>0.68</v>
+        <v>0.67800000000000005</v>
       </c>
       <c r="D7" t="s">
         <v>34</v>
       </c>
       <c r="E7" s="1">
-        <v>0.38</v>
+        <v>0.753</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="G7" s="1">
-        <v>0.26500000000000001</v>
+        <v>0.46700000000000003</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="P7">
-        <v>0.95389999999999997</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="R7">
-        <v>0.72829999999999995</v>
-      </c>
-      <c r="S7" t="s">
-        <v>67</v>
-      </c>
-      <c r="T7" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C8" s="1">
+        <v>0.68</v>
+      </c>
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.38</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="P8">
+        <v>0.95389999999999997</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R8">
+        <v>0.72829999999999995</v>
+      </c>
+      <c r="S8" t="s">
+        <v>66</v>
+      </c>
+      <c r="T8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="1">
         <v>0.38435399999999997</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H8" s="1" t="s">
+      <c r="I9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J8" s="1" t="s">
+      <c r="K9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L9" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="K8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L8" s="1" t="s">
+      <c r="M9" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="M8" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B14" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.35">
@@ -1318,22 +1359,22 @@
         <v>1</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D16" t="s">
         <v>17</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F16" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="I16" t="s">
         <v>22</v>
@@ -1345,28 +1386,28 @@
         <v>25</v>
       </c>
       <c r="L16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M16" t="s">
+        <v>103</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="O16" t="s">
         <v>105</v>
       </c>
-      <c r="N16" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="O16" t="s">
-        <v>107</v>
-      </c>
       <c r="P16" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="Q16" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="S16" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="R16" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="S16" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="T16" t="s">
         <v>22</v>
@@ -1377,31 +1418,28 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>4</v>
+        <v>121</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>79</v>
+        <v>122</v>
       </c>
       <c r="C17" s="1">
-        <v>0.28799999999999998</v>
+        <v>0.191</v>
       </c>
       <c r="D17" t="s">
         <v>34</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="F17" s="1">
-        <v>0.90847259999999996</v>
+        <v>0.53714859999999998</v>
       </c>
       <c r="G17" s="1">
-        <v>0.59664039999999996</v>
+        <v>0.84018139999999997</v>
       </c>
       <c r="H17" s="1">
-        <v>0.31416110000000003</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>33</v>
+        <v>0.16666590000000001</v>
+      </c>
+      <c r="I17" t="s">
+        <v>123</v>
       </c>
       <c r="J17" t="s">
         <v>33</v>
@@ -1409,28 +1447,28 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>94</v>
+        <v>122</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.28799999999999998</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F18" s="1">
-        <v>0.21866269999999999</v>
+        <v>0.90847259999999996</v>
       </c>
       <c r="G18" s="1">
-        <v>0.61769870000000004</v>
+        <v>0.59664039999999996</v>
       </c>
       <c r="H18" s="1">
-        <v>1.6265399999999999E-2</v>
+        <v>0.31416110000000003</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>33</v>
@@ -1441,31 +1479,31 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C19" s="1">
-        <v>0.29299999999999998</v>
+        <v>122</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="D19" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F19" s="1">
-        <v>0.96322099999999999</v>
+        <v>0.21866269999999999</v>
       </c>
       <c r="G19" s="1">
-        <v>0.3518867</v>
+        <v>0.61769870000000004</v>
       </c>
       <c r="H19" s="1">
-        <v>0.52779640000000005</v>
+        <v>1.6265399999999999E-2</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J19" t="s">
         <v>33</v>
@@ -1473,245 +1511,240 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>79</v>
+        <v>122</v>
       </c>
       <c r="C20" s="1">
-        <v>0.438</v>
+        <v>0.29299999999999998</v>
       </c>
       <c r="D20" t="s">
         <v>34</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F20" s="1">
-        <v>0.95264649999999995</v>
+        <v>0.96322099999999999</v>
       </c>
       <c r="G20" s="1">
-        <v>0.69391789999999998</v>
+        <v>0.3518867</v>
       </c>
       <c r="H20" s="1">
-        <v>0.47374840000000001</v>
+        <v>0.52779640000000005</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>34</v>
       </c>
       <c r="J20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>79</v>
+        <v>122</v>
       </c>
       <c r="C21" s="1">
-        <v>0.92</v>
+        <v>0.438</v>
       </c>
       <c r="D21" t="s">
         <v>34</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F21" s="1">
-        <v>0.98473310000000003</v>
+        <v>0.95264649999999995</v>
       </c>
       <c r="G21" s="1">
-        <v>0.98015640000000004</v>
+        <v>0.69391789999999998</v>
       </c>
       <c r="H21" s="1">
-        <v>0.91700090000000001</v>
+        <v>0.47374840000000001</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J21" t="s">
-        <v>33</v>
-      </c>
-      <c r="L21" t="s">
-        <v>14</v>
-      </c>
-      <c r="M21" t="s">
-        <v>109</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>79</v>
+        <v>122</v>
       </c>
       <c r="C22" s="1">
-        <v>0.46600000000000003</v>
+        <v>0.92</v>
       </c>
       <c r="D22" t="s">
         <v>34</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F22" s="1">
-        <v>0.99019550000000001</v>
+        <v>0.98473310000000003</v>
       </c>
       <c r="G22" s="1">
-        <v>0.54496310000000003</v>
+        <v>0.98015640000000004</v>
       </c>
       <c r="H22" s="1">
-        <v>0.64525869999999996</v>
+        <v>0.91700090000000001</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J22" t="s">
-        <v>111</v>
+        <v>33</v>
+      </c>
+      <c r="L22" t="s">
+        <v>14</v>
+      </c>
+      <c r="M22" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="D23" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0.99019550000000001</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0.54496310000000003</v>
+      </c>
+      <c r="H23" s="1">
+        <v>0.64525869999999996</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J23" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C23" s="1" t="s">
+      <c r="B24" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F24" s="1">
+        <v>0.84509029999999996</v>
+      </c>
+      <c r="G24" s="1">
+        <v>1.0333999999999999E-2</v>
+      </c>
+      <c r="H24" s="1">
+        <v>4.3346500000000003E-2</v>
+      </c>
+      <c r="I24" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D23" t="s">
-        <v>14</v>
-      </c>
-      <c r="E23" s="1" t="s">
+      <c r="J24" t="s">
         <v>119</v>
       </c>
-      <c r="F23" s="1">
-        <v>0.84509029999999996</v>
-      </c>
-      <c r="G23" s="1">
-        <v>1.0333999999999999E-2</v>
-      </c>
-      <c r="H23" s="1">
-        <v>4.3346500000000003E-2</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="J23" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B25" s="1" t="s">
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B26" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B28" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" t="s">
+        <v>84</v>
+      </c>
+      <c r="E28" t="s">
+        <v>83</v>
+      </c>
+      <c r="F28" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B27" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="G28" t="s">
+        <v>22</v>
+      </c>
+      <c r="H28" t="s">
+        <v>21</v>
+      </c>
+      <c r="I28" t="s">
+        <v>85</v>
+      </c>
+      <c r="J28" t="s">
+        <v>25</v>
+      </c>
+      <c r="K28" t="s">
+        <v>37</v>
+      </c>
+      <c r="L28" t="s">
+        <v>91</v>
+      </c>
+      <c r="M28" t="s">
         <v>86</v>
       </c>
-      <c r="E27" t="s">
-        <v>85</v>
-      </c>
-      <c r="F27" t="s">
-        <v>78</v>
-      </c>
-      <c r="G27" t="s">
-        <v>22</v>
-      </c>
-      <c r="H27" t="s">
-        <v>21</v>
-      </c>
-      <c r="I27" t="s">
-        <v>87</v>
-      </c>
-      <c r="J27" t="s">
-        <v>25</v>
-      </c>
-      <c r="K27" t="s">
-        <v>38</v>
-      </c>
-      <c r="L27" t="s">
-        <v>93</v>
-      </c>
-      <c r="M27" t="s">
-        <v>88</v>
-      </c>
-      <c r="N27" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="O27" s="1" t="s">
+      <c r="N28" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="P28" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q28" t="s">
         <v>115</v>
       </c>
-      <c r="P27" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>4</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C28" s="1">
-        <v>0.37009999999999998</v>
-      </c>
-      <c r="D28" s="1">
-        <v>0.13519999999999999</v>
-      </c>
-      <c r="E28" s="1">
-        <v>-8.8990000000000007E-3</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="I28" t="s">
-        <v>34</v>
-      </c>
-      <c r="J28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
-      <c r="N28" t="s">
-        <v>90</v>
-      </c>
-      <c r="O28"/>
-      <c r="P28" s="2"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>5</v>
+        <v>121</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C29" s="1">
-        <v>0.30270000000000002</v>
+        <v>0.84609999999999996</v>
       </c>
       <c r="D29" s="1">
-        <v>0.17480000000000001</v>
+        <v>6.8009999999999998E-3</v>
       </c>
       <c r="E29" s="1">
-        <v>3.7249999999999998E-2</v>
+        <v>-0.15870000000000001</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>34</v>
@@ -1720,45 +1753,30 @@
         <v>33</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>100</v>
+        <v>34</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="L29" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="N29" t="s">
-        <v>101</v>
-      </c>
-      <c r="O29">
-        <v>0.26729999999999998</v>
-      </c>
-      <c r="P29" s="2">
-        <v>0.19950000000000001</v>
-      </c>
-      <c r="Q29">
-        <v>6.6030000000000005E-2</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C30" s="1">
-        <v>0.88749999999999996</v>
+        <v>0.37009999999999998</v>
       </c>
       <c r="D30" s="1">
-        <v>3.62E-3</v>
+        <v>0.13519999999999999</v>
       </c>
       <c r="E30" s="1">
-        <v>-0.16239999999999999</v>
+        <v>-8.8990000000000007E-3</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>34</v>
@@ -1767,48 +1785,37 @@
         <v>33</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="I30" t="s">
-        <v>102</v>
+        <v>34</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="L30" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M30" t="s">
-        <v>14</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
       <c r="N30" t="s">
-        <v>104</v>
-      </c>
-      <c r="O30">
-        <v>0.83540000000000003</v>
-      </c>
-      <c r="P30" s="2">
-        <v>7.783E-3</v>
-      </c>
-      <c r="Q30">
-        <v>-0.15759999999999999</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="O30"/>
+      <c r="P30" s="2"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C31" s="1">
-        <v>0.87009999999999998</v>
+        <v>0.30270000000000002</v>
       </c>
       <c r="D31" s="1">
-        <v>4.8269999999999997E-3</v>
+        <v>0.17480000000000001</v>
       </c>
       <c r="E31" s="1">
-        <v>-0.161</v>
+        <v>3.7249999999999998E-2</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>34</v>
@@ -1817,32 +1824,45 @@
         <v>33</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="I31" t="s">
-        <v>100</v>
+        <v>97</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="N31" t="s">
-        <v>92</v>
-      </c>
-      <c r="O31"/>
-      <c r="P31" s="2"/>
+        <v>99</v>
+      </c>
+      <c r="O31">
+        <v>0.26729999999999998</v>
+      </c>
+      <c r="P31" s="2">
+        <v>0.19950000000000001</v>
+      </c>
+      <c r="Q31">
+        <v>6.6030000000000005E-2</v>
+      </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C32" s="1">
-        <v>0.87909999999999999</v>
+        <v>0.88749999999999996</v>
       </c>
       <c r="D32" s="1">
-        <v>4.1799999999999997E-3</v>
+        <v>3.62E-3</v>
       </c>
       <c r="E32" s="1">
-        <v>-0.1618</v>
+        <v>-0.16239999999999999</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>34</v>
@@ -1851,106 +1871,190 @@
         <v>33</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>110</v>
+        <v>101</v>
+      </c>
+      <c r="I32" t="s">
+        <v>100</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M32" t="s">
+        <v>14</v>
       </c>
       <c r="N32" t="s">
-        <v>92</v>
-      </c>
-      <c r="O32"/>
-      <c r="P32" s="2"/>
+        <v>102</v>
+      </c>
+      <c r="O32">
+        <v>0.83540000000000003</v>
+      </c>
+      <c r="P32" s="2">
+        <v>7.783E-3</v>
+      </c>
+      <c r="Q32">
+        <v>-0.15759999999999999</v>
+      </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C33" s="1">
-        <v>0.39</v>
+        <v>0.87009999999999998</v>
       </c>
       <c r="D33" s="1">
-        <v>0.12509999999999999</v>
+        <v>4.8269999999999997E-3</v>
       </c>
       <c r="E33" s="1">
-        <v>-2.069E-2</v>
+        <v>-0.161</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>34</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>114</v>
+        <v>33</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="I33" t="s">
-        <v>102</v>
-      </c>
-      <c r="J33" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="L33" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="M33" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
       <c r="N33" t="s">
-        <v>92</v>
-      </c>
-      <c r="O33">
-        <v>0.37830000000000003</v>
-      </c>
-      <c r="P33" s="2">
-        <v>0.13100000000000001</v>
-      </c>
-      <c r="Q33">
-        <v>-1.3820000000000001E-2</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="O33"/>
+      <c r="P33" s="2"/>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C34" s="1">
-        <v>6.0060000000000002E-2</v>
+        <v>0.87909999999999999</v>
       </c>
       <c r="D34" s="1">
-        <v>0.4713</v>
+        <v>4.1799999999999997E-3</v>
       </c>
       <c r="E34" s="1">
-        <v>0.3831</v>
+        <v>-0.1618</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I34" t="s">
-        <v>102</v>
-      </c>
-      <c r="J34" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="L34" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I34" s="1" t="s">
         <v>108</v>
       </c>
       <c r="N34" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="O34"/>
       <c r="P34" s="2"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C35" s="1">
+        <v>0.39</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0.12509999999999999</v>
+      </c>
+      <c r="E35" s="1">
+        <v>-2.069E-2</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I35" t="s">
+        <v>100</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="M35" t="s">
+        <v>34</v>
+      </c>
+      <c r="N35" t="s">
+        <v>90</v>
+      </c>
+      <c r="O35">
+        <v>0.37830000000000003</v>
+      </c>
+      <c r="P35" s="2">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="Q35">
+        <v>-1.3820000000000001E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" s="1">
+        <v>6.0060000000000002E-2</v>
+      </c>
+      <c r="D36" s="1">
+        <v>0.4713</v>
+      </c>
+      <c r="E36" s="1">
+        <v>0.3831</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I36" t="s">
+        <v>100</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="N36" t="s">
+        <v>90</v>
+      </c>
+      <c r="O36"/>
+      <c r="P36" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>